<commit_message>
Updated the blank RO spreadsheet with new values
</commit_message>
<xml_diff>
--- a/spec/support/blankRoSpreadsheet.xlsx
+++ b/spec/support/blankRoSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomas/Desktop/tmp/compare/redone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A847F8-1B79-E945-AB72-C18C9EA6B8DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62C634A-52C8-384D-85B9-EA611D61B46E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="1100" windowWidth="17980" windowHeight="20620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="123">
   <si>
     <t>Example</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
+  </si>
+  <si>
+    <t>Number of Hearing Days Without Rooms in Date Range</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -512,7 +515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -749,19 +752,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -942,11 +932,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1001,16 +1019,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1026,9 +1044,6 @@
     <xf numFmtId="14" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1044,26 +1059,26 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1076,10 +1091,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2274,9 +2295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IT50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
@@ -2287,24 +2308,24 @@
     <col min="7" max="254" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="56" customHeight="1">
+    <row r="1" spans="1:57" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2350,7 +2371,7 @@
       <c r="BD1" s="4"/>
       <c r="BE1" s="5"/>
     </row>
-    <row r="2" spans="1:57" ht="39" customHeight="1">
+    <row r="2" spans="1:57" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2523,7 +2544,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:57" ht="34" customHeight="1">
+    <row r="3" spans="1:57" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2696,7 +2717,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:57" ht="32" customHeight="1">
+    <row r="4" spans="1:57" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2869,7 +2890,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="17" customHeight="1">
+    <row r="5" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="20">
         <v>43497</v>
@@ -2930,7 +2951,7 @@
       <c r="BD5" s="22"/>
       <c r="BE5" s="22"/>
     </row>
-    <row r="6" spans="1:57" ht="17" customHeight="1">
+    <row r="6" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="23">
         <v>43540</v>
@@ -2991,7 +3012,7 @@
       <c r="BD6" s="22"/>
       <c r="BE6" s="22"/>
     </row>
-    <row r="7" spans="1:57" ht="17" customHeight="1">
+    <row r="7" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="24">
         <v>43576</v>
@@ -3052,7 +3073,7 @@
       <c r="BD7" s="22"/>
       <c r="BE7" s="22"/>
     </row>
-    <row r="8" spans="1:57" ht="17" customHeight="1">
+    <row r="8" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="26">
         <v>43604</v>
@@ -3113,7 +3134,7 @@
       <c r="BD8" s="29"/>
       <c r="BE8" s="29"/>
     </row>
-    <row r="9" spans="1:57" ht="17" customHeight="1">
+    <row r="9" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -3172,7 +3193,7 @@
       <c r="BD9" s="29"/>
       <c r="BE9" s="29"/>
     </row>
-    <row r="10" spans="1:57" ht="17" customHeight="1">
+    <row r="10" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
@@ -3231,7 +3252,7 @@
       <c r="BD10" s="28"/>
       <c r="BE10" s="28"/>
     </row>
-    <row r="11" spans="1:57" ht="17" customHeight="1">
+    <row r="11" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="34"/>
       <c r="C11" s="31"/>
@@ -3290,7 +3311,7 @@
       <c r="BD11" s="31"/>
       <c r="BE11" s="35"/>
     </row>
-    <row r="12" spans="1:57" ht="17" customHeight="1">
+    <row r="12" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="32"/>
       <c r="C12" s="33"/>
@@ -3349,7 +3370,7 @@
       <c r="BD12" s="33"/>
       <c r="BE12" s="33"/>
     </row>
-    <row r="13" spans="1:57" ht="17" customHeight="1">
+    <row r="13" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="34"/>
       <c r="C13" s="36"/>
@@ -3408,7 +3429,7 @@
       <c r="BD13" s="36"/>
       <c r="BE13" s="37"/>
     </row>
-    <row r="14" spans="1:57" ht="17" customHeight="1">
+    <row r="14" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="32"/>
       <c r="C14" s="38"/>
@@ -3467,7 +3488,7 @@
       <c r="BD14" s="38"/>
       <c r="BE14" s="38"/>
     </row>
-    <row r="15" spans="1:57" ht="17" customHeight="1">
+    <row r="15" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="34"/>
       <c r="C15" s="36"/>
@@ -3526,7 +3547,7 @@
       <c r="BD15" s="36"/>
       <c r="BE15" s="37"/>
     </row>
-    <row r="16" spans="1:57" ht="17" customHeight="1">
+    <row r="16" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="32"/>
       <c r="C16" s="38"/>
@@ -3585,7 +3606,7 @@
       <c r="BD16" s="38"/>
       <c r="BE16" s="38"/>
     </row>
-    <row r="17" spans="1:57" ht="17" customHeight="1">
+    <row r="17" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="34"/>
       <c r="C17" s="36"/>
@@ -3644,7 +3665,7 @@
       <c r="BD17" s="36"/>
       <c r="BE17" s="37"/>
     </row>
-    <row r="18" spans="1:57" ht="17" customHeight="1">
+    <row r="18" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="32"/>
       <c r="C18" s="38"/>
@@ -3703,7 +3724,7 @@
       <c r="BD18" s="38"/>
       <c r="BE18" s="38"/>
     </row>
-    <row r="19" spans="1:57" ht="17" customHeight="1">
+    <row r="19" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -3762,7 +3783,7 @@
       <c r="BD19" s="36"/>
       <c r="BE19" s="37"/>
     </row>
-    <row r="20" spans="1:57" ht="17" customHeight="1">
+    <row r="20" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="32"/>
       <c r="C20" s="38"/>
@@ -3821,7 +3842,7 @@
       <c r="BD20" s="38"/>
       <c r="BE20" s="38"/>
     </row>
-    <row r="21" spans="1:57" ht="17" customHeight="1">
+    <row r="21" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="34"/>
       <c r="C21" s="36"/>
@@ -3880,7 +3901,7 @@
       <c r="BD21" s="36"/>
       <c r="BE21" s="37"/>
     </row>
-    <row r="22" spans="1:57" ht="17" customHeight="1">
+    <row r="22" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="32"/>
       <c r="C22" s="38"/>
@@ -3939,7 +3960,7 @@
       <c r="BD22" s="38"/>
       <c r="BE22" s="38"/>
     </row>
-    <row r="23" spans="1:57" ht="17" customHeight="1">
+    <row r="23" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="34"/>
       <c r="C23" s="36"/>
@@ -3998,7 +4019,7 @@
       <c r="BD23" s="36"/>
       <c r="BE23" s="37"/>
     </row>
-    <row r="24" spans="1:57" ht="17" customHeight="1">
+    <row r="24" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="32"/>
       <c r="C24" s="38"/>
@@ -4057,7 +4078,7 @@
       <c r="BD24" s="38"/>
       <c r="BE24" s="38"/>
     </row>
-    <row r="25" spans="1:57" ht="17" customHeight="1">
+    <row r="25" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="34"/>
       <c r="C25" s="36"/>
@@ -4116,7 +4137,7 @@
       <c r="BD25" s="36"/>
       <c r="BE25" s="37"/>
     </row>
-    <row r="26" spans="1:57" ht="17" customHeight="1">
+    <row r="26" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="32"/>
       <c r="C26" s="38"/>
@@ -4175,7 +4196,7 @@
       <c r="BD26" s="38"/>
       <c r="BE26" s="38"/>
     </row>
-    <row r="27" spans="1:57" ht="17" customHeight="1">
+    <row r="27" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="34"/>
       <c r="C27" s="36"/>
@@ -4234,7 +4255,7 @@
       <c r="BD27" s="36"/>
       <c r="BE27" s="37"/>
     </row>
-    <row r="28" spans="1:57" ht="17" customHeight="1">
+    <row r="28" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="32"/>
       <c r="C28" s="38"/>
@@ -4293,7 +4314,7 @@
       <c r="BD28" s="38"/>
       <c r="BE28" s="38"/>
     </row>
-    <row r="29" spans="1:57" ht="17" customHeight="1">
+    <row r="29" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="34"/>
       <c r="C29" s="36"/>
@@ -4352,7 +4373,7 @@
       <c r="BD29" s="36"/>
       <c r="BE29" s="37"/>
     </row>
-    <row r="30" spans="1:57" ht="17" customHeight="1">
+    <row r="30" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="32"/>
       <c r="C30" s="38"/>
@@ -4411,7 +4432,7 @@
       <c r="BD30" s="38"/>
       <c r="BE30" s="38"/>
     </row>
-    <row r="31" spans="1:57" ht="17" customHeight="1">
+    <row r="31" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="34"/>
       <c r="C31" s="36"/>
@@ -4470,7 +4491,7 @@
       <c r="BD31" s="36"/>
       <c r="BE31" s="37"/>
     </row>
-    <row r="32" spans="1:57" ht="17" customHeight="1">
+    <row r="32" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="32"/>
       <c r="C32" s="38"/>
@@ -4529,7 +4550,7 @@
       <c r="BD32" s="38"/>
       <c r="BE32" s="38"/>
     </row>
-    <row r="33" spans="1:57" ht="17" customHeight="1">
+    <row r="33" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" s="34"/>
       <c r="C33" s="36"/>
@@ -4588,7 +4609,7 @@
       <c r="BD33" s="36"/>
       <c r="BE33" s="37"/>
     </row>
-    <row r="34" spans="1:57" ht="17" customHeight="1">
+    <row r="34" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="32"/>
       <c r="C34" s="38"/>
@@ -4647,7 +4668,7 @@
       <c r="BD34" s="38"/>
       <c r="BE34" s="38"/>
     </row>
-    <row r="35" spans="1:57" ht="17" customHeight="1">
+    <row r="35" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
       <c r="B35" s="34"/>
       <c r="C35" s="36"/>
@@ -4706,7 +4727,7 @@
       <c r="BD35" s="36"/>
       <c r="BE35" s="37"/>
     </row>
-    <row r="36" spans="1:57" ht="17" customHeight="1">
+    <row r="36" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="32"/>
       <c r="C36" s="38"/>
@@ -4765,7 +4786,7 @@
       <c r="BD36" s="38"/>
       <c r="BE36" s="38"/>
     </row>
-    <row r="37" spans="1:57" ht="17" customHeight="1">
+    <row r="37" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="34"/>
       <c r="C37" s="36"/>
@@ -4824,7 +4845,7 @@
       <c r="BD37" s="36"/>
       <c r="BE37" s="37"/>
     </row>
-    <row r="38" spans="1:57" ht="17" customHeight="1">
+    <row r="38" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
       <c r="B38" s="32"/>
       <c r="C38" s="38"/>
@@ -4883,7 +4904,7 @@
       <c r="BD38" s="38"/>
       <c r="BE38" s="38"/>
     </row>
-    <row r="39" spans="1:57" ht="17" customHeight="1">
+    <row r="39" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
       <c r="B39" s="34"/>
       <c r="C39" s="36"/>
@@ -4942,7 +4963,7 @@
       <c r="BD39" s="36"/>
       <c r="BE39" s="37"/>
     </row>
-    <row r="40" spans="1:57" ht="17" customHeight="1">
+    <row r="40" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19"/>
       <c r="B40" s="32"/>
       <c r="C40" s="38"/>
@@ -5001,7 +5022,7 @@
       <c r="BD40" s="38"/>
       <c r="BE40" s="38"/>
     </row>
-    <row r="41" spans="1:57" ht="17" customHeight="1">
+    <row r="41" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="34"/>
       <c r="C41" s="36"/>
@@ -5060,7 +5081,7 @@
       <c r="BD41" s="36"/>
       <c r="BE41" s="37"/>
     </row>
-    <row r="42" spans="1:57" ht="17" customHeight="1">
+    <row r="42" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="32"/>
       <c r="C42" s="38"/>
@@ -5119,7 +5140,7 @@
       <c r="BD42" s="38"/>
       <c r="BE42" s="38"/>
     </row>
-    <row r="43" spans="1:57" ht="17" customHeight="1">
+    <row r="43" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="34"/>
       <c r="C43" s="36"/>
@@ -5178,7 +5199,7 @@
       <c r="BD43" s="36"/>
       <c r="BE43" s="37"/>
     </row>
-    <row r="44" spans="1:57" ht="17" customHeight="1">
+    <row r="44" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="32"/>
       <c r="C44" s="38"/>
@@ -5237,7 +5258,7 @@
       <c r="BD44" s="38"/>
       <c r="BE44" s="38"/>
     </row>
-    <row r="45" spans="1:57" ht="17" customHeight="1">
+    <row r="45" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="34"/>
       <c r="C45" s="36"/>
@@ -5296,7 +5317,7 @@
       <c r="BD45" s="36"/>
       <c r="BE45" s="37"/>
     </row>
-    <row r="46" spans="1:57" ht="17" customHeight="1">
+    <row r="46" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="32"/>
       <c r="C46" s="38"/>
@@ -5355,7 +5376,7 @@
       <c r="BD46" s="38"/>
       <c r="BE46" s="38"/>
     </row>
-    <row r="47" spans="1:57" ht="17" customHeight="1">
+    <row r="47" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="34"/>
       <c r="C47" s="36"/>
@@ -5414,7 +5435,7 @@
       <c r="BD47" s="36"/>
       <c r="BE47" s="37"/>
     </row>
-    <row r="48" spans="1:57" ht="17" customHeight="1">
+    <row r="48" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="32"/>
       <c r="C48" s="38"/>
@@ -5473,7 +5494,7 @@
       <c r="BD48" s="38"/>
       <c r="BE48" s="38"/>
     </row>
-    <row r="49" spans="1:57" ht="17" customHeight="1">
+    <row r="49" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
       <c r="B49" s="34"/>
       <c r="C49" s="36"/>
@@ -5532,7 +5553,7 @@
       <c r="BD49" s="36"/>
       <c r="BE49" s="37"/>
     </row>
-    <row r="50" spans="1:57" ht="17" customHeight="1">
+    <row r="50" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="39"/>
       <c r="B50" s="40"/>
       <c r="C50" s="41"/>
@@ -5611,23 +5632,23 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="42" customWidth="1"/>
     <col min="2" max="2" width="48" style="42" customWidth="1"/>
     <col min="3" max="256" width="8.6640625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="73"/>
       <c r="C1" s="43"/>
       <c r="D1" s="44"/>
       <c r="E1" s="44"/>
     </row>
-    <row r="2" spans="1:5" ht="43.5" customHeight="1">
+    <row r="2" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45"/>
       <c r="B2" s="46" t="s">
         <v>116</v>
@@ -5636,7 +5657,7 @@
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
     </row>
-    <row r="3" spans="1:5" ht="36.75" customHeight="1">
+    <row r="3" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>0</v>
       </c>
@@ -5647,7 +5668,7 @@
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
     </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="17" t="s">
         <v>117</v>
@@ -5656,42 +5677,42 @@
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
     </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="44"/>
       <c r="B5" s="22"/>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
       <c r="E5" s="44"/>
     </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44"/>
       <c r="B6" s="22"/>
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="44"/>
       <c r="B7" s="22"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
     </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44"/>
       <c r="B8" s="25"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
       <c r="E8" s="44"/>
     </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
       <c r="E9" s="44"/>
     </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -5714,50 +5735,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV97"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="50" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="50" customWidth="1"/>
     <col min="3" max="3" width="11" style="50" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="50" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="50" customWidth="1"/>
+    <col min="5" max="5" width="23" style="77" customWidth="1"/>
     <col min="6" max="256" width="11" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="60" customHeight="1">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-    </row>
-    <row r="2" spans="1:14" ht="47" customHeight="1">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+    </row>
+    <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="43"/>
+      <c r="E2" s="55" t="s">
+        <v>122</v>
+      </c>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -5768,20 +5791,22 @@
       <c r="M2" s="44"/>
       <c r="N2" s="44"/>
     </row>
-    <row r="3" spans="1:14" ht="39" customHeight="1">
-      <c r="A3" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="58" t="s">
+    <row r="3" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="60">
+      <c r="D3" s="59">
         <v>10</v>
       </c>
-      <c r="E3" s="43"/>
+      <c r="E3" s="75">
+        <v>50</v>
+      </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
@@ -5792,18 +5817,20 @@
       <c r="M3" s="44"/>
       <c r="N3" s="44"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62" t="s">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="60"/>
+      <c r="B4" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="64">
-        <v>0</v>
-      </c>
-      <c r="E4" s="43"/>
+      <c r="D4" s="63">
+        <v>0</v>
+      </c>
+      <c r="E4" s="63">
+        <v>0</v>
+      </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
@@ -5814,18 +5841,20 @@
       <c r="M4" s="44"/>
       <c r="N4" s="44"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="62" t="s">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="64"/>
+      <c r="B5" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="64">
-        <v>0</v>
-      </c>
-      <c r="E5" s="43"/>
+      <c r="D5" s="63">
+        <v>0</v>
+      </c>
+      <c r="E5" s="63">
+        <v>0</v>
+      </c>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
@@ -5836,18 +5865,20 @@
       <c r="M5" s="44"/>
       <c r="N5" s="44"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A6" s="66"/>
-      <c r="B6" s="62" t="s">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="65"/>
+      <c r="B6" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="64">
-        <v>0</v>
-      </c>
-      <c r="E6" s="43"/>
+      <c r="D6" s="63">
+        <v>0</v>
+      </c>
+      <c r="E6" s="63">
+        <v>0</v>
+      </c>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
@@ -5858,18 +5889,20 @@
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A7" s="67"/>
-      <c r="B7" s="62" t="s">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="66"/>
+      <c r="B7" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="64">
-        <v>0</v>
-      </c>
-      <c r="E7" s="43"/>
+      <c r="D7" s="63">
+        <v>0</v>
+      </c>
+      <c r="E7" s="63">
+        <v>0</v>
+      </c>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
@@ -5880,18 +5913,20 @@
       <c r="M7" s="44"/>
       <c r="N7" s="44"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A8" s="67"/>
-      <c r="B8" s="62" t="s">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="66"/>
+      <c r="B8" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="64">
-        <v>0</v>
-      </c>
-      <c r="E8" s="43"/>
+      <c r="D8" s="63">
+        <v>0</v>
+      </c>
+      <c r="E8" s="63">
+        <v>0</v>
+      </c>
       <c r="F8" s="44"/>
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
@@ -5902,18 +5937,20 @@
       <c r="M8" s="44"/>
       <c r="N8" s="44"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A9" s="67"/>
-      <c r="B9" s="62" t="s">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="66"/>
+      <c r="B9" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="64">
-        <v>0</v>
-      </c>
-      <c r="E9" s="43"/>
+      <c r="D9" s="63">
+        <v>0</v>
+      </c>
+      <c r="E9" s="63">
+        <v>0</v>
+      </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44"/>
       <c r="H9" s="44"/>
@@ -5924,18 +5961,20 @@
       <c r="M9" s="44"/>
       <c r="N9" s="44"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A10" s="67"/>
-      <c r="B10" s="62" t="s">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="66"/>
+      <c r="B10" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="64">
-        <v>0</v>
-      </c>
-      <c r="E10" s="43"/>
+      <c r="D10" s="63">
+        <v>0</v>
+      </c>
+      <c r="E10" s="63">
+        <v>0</v>
+      </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44"/>
       <c r="H10" s="44"/>
@@ -5946,18 +5985,20 @@
       <c r="M10" s="44"/>
       <c r="N10" s="44"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="62" t="s">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="66"/>
+      <c r="B11" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="64">
-        <v>0</v>
-      </c>
-      <c r="E11" s="43"/>
+      <c r="D11" s="63">
+        <v>0</v>
+      </c>
+      <c r="E11" s="63">
+        <v>0</v>
+      </c>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
@@ -5968,18 +6009,20 @@
       <c r="M11" s="44"/>
       <c r="N11" s="44"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A12" s="67"/>
-      <c r="B12" s="62" t="s">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="66"/>
+      <c r="B12" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="64">
-        <v>0</v>
-      </c>
-      <c r="E12" s="43"/>
+      <c r="D12" s="63">
+        <v>0</v>
+      </c>
+      <c r="E12" s="63">
+        <v>0</v>
+      </c>
       <c r="F12" s="44"/>
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
@@ -5990,18 +6033,20 @@
       <c r="M12" s="44"/>
       <c r="N12" s="44"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A13" s="67"/>
-      <c r="B13" s="62" t="s">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="66"/>
+      <c r="B13" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="64">
-        <v>0</v>
-      </c>
-      <c r="E13" s="43"/>
+      <c r="D13" s="63">
+        <v>0</v>
+      </c>
+      <c r="E13" s="63">
+        <v>0</v>
+      </c>
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
@@ -6012,18 +6057,20 @@
       <c r="M13" s="44"/>
       <c r="N13" s="44"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A14" s="67"/>
-      <c r="B14" s="62" t="s">
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="66"/>
+      <c r="B14" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="64">
-        <v>0</v>
-      </c>
-      <c r="E14" s="43"/>
+      <c r="D14" s="63">
+        <v>0</v>
+      </c>
+      <c r="E14" s="63">
+        <v>0</v>
+      </c>
       <c r="F14" s="44"/>
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
@@ -6034,18 +6081,20 @@
       <c r="M14" s="44"/>
       <c r="N14" s="44"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A15" s="67"/>
-      <c r="B15" s="62" t="s">
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="66"/>
+      <c r="B15" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="64">
-        <v>0</v>
-      </c>
-      <c r="E15" s="43"/>
+      <c r="D15" s="63">
+        <v>0</v>
+      </c>
+      <c r="E15" s="63">
+        <v>0</v>
+      </c>
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
       <c r="H15" s="44"/>
@@ -6056,18 +6105,20 @@
       <c r="M15" s="44"/>
       <c r="N15" s="44"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A16" s="67"/>
-      <c r="B16" s="62" t="s">
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="66"/>
+      <c r="B16" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="64">
-        <v>0</v>
-      </c>
-      <c r="E16" s="43"/>
+      <c r="D16" s="63">
+        <v>0</v>
+      </c>
+      <c r="E16" s="63">
+        <v>0</v>
+      </c>
       <c r="F16" s="44"/>
       <c r="G16" s="44"/>
       <c r="H16" s="44"/>
@@ -6078,18 +6129,20 @@
       <c r="M16" s="44"/>
       <c r="N16" s="44"/>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="67"/>
-      <c r="B17" s="62" t="s">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="66"/>
+      <c r="B17" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="64">
-        <v>0</v>
-      </c>
-      <c r="E17" s="43"/>
+      <c r="D17" s="63">
+        <v>0</v>
+      </c>
+      <c r="E17" s="63">
+        <v>0</v>
+      </c>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
@@ -6100,18 +6153,20 @@
       <c r="M17" s="44"/>
       <c r="N17" s="44"/>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A18" s="67"/>
-      <c r="B18" s="62" t="s">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="66"/>
+      <c r="B18" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="64">
-        <v>0</v>
-      </c>
-      <c r="E18" s="43"/>
+      <c r="D18" s="63">
+        <v>0</v>
+      </c>
+      <c r="E18" s="63">
+        <v>0</v>
+      </c>
       <c r="F18" s="44"/>
       <c r="G18" s="44"/>
       <c r="H18" s="44"/>
@@ -6122,18 +6177,20 @@
       <c r="M18" s="44"/>
       <c r="N18" s="44"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A19" s="67"/>
-      <c r="B19" s="62" t="s">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="66"/>
+      <c r="B19" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="64">
-        <v>0</v>
-      </c>
-      <c r="E19" s="43"/>
+      <c r="D19" s="63">
+        <v>0</v>
+      </c>
+      <c r="E19" s="63">
+        <v>0</v>
+      </c>
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
@@ -6144,18 +6201,20 @@
       <c r="M19" s="44"/>
       <c r="N19" s="44"/>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A20" s="67"/>
-      <c r="B20" s="62" t="s">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="66"/>
+      <c r="B20" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="63" t="s">
+      <c r="C20" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="64">
-        <v>0</v>
-      </c>
-      <c r="E20" s="43"/>
+      <c r="D20" s="63">
+        <v>0</v>
+      </c>
+      <c r="E20" s="63">
+        <v>0</v>
+      </c>
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
@@ -6166,18 +6225,20 @@
       <c r="M20" s="44"/>
       <c r="N20" s="44"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A21" s="67"/>
-      <c r="B21" s="62" t="s">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="66"/>
+      <c r="B21" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="64">
-        <v>0</v>
-      </c>
-      <c r="E21" s="43"/>
+      <c r="D21" s="63">
+        <v>0</v>
+      </c>
+      <c r="E21" s="63">
+        <v>0</v>
+      </c>
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
       <c r="H21" s="44"/>
@@ -6188,18 +6249,20 @@
       <c r="M21" s="44"/>
       <c r="N21" s="44"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A22" s="67"/>
-      <c r="B22" s="62" t="s">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="66"/>
+      <c r="B22" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="64">
-        <v>0</v>
-      </c>
-      <c r="E22" s="43"/>
+      <c r="D22" s="63">
+        <v>0</v>
+      </c>
+      <c r="E22" s="63">
+        <v>0</v>
+      </c>
       <c r="F22" s="44"/>
       <c r="G22" s="44"/>
       <c r="H22" s="44"/>
@@ -6210,18 +6273,20 @@
       <c r="M22" s="44"/>
       <c r="N22" s="44"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A23" s="67"/>
-      <c r="B23" s="62" t="s">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="66"/>
+      <c r="B23" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="64">
-        <v>0</v>
-      </c>
-      <c r="E23" s="43"/>
+      <c r="D23" s="63">
+        <v>0</v>
+      </c>
+      <c r="E23" s="63">
+        <v>0</v>
+      </c>
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
@@ -6232,18 +6297,20 @@
       <c r="M23" s="44"/>
       <c r="N23" s="44"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="67"/>
-      <c r="B24" s="62" t="s">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="66"/>
+      <c r="B24" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="C24" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="64">
-        <v>0</v>
-      </c>
-      <c r="E24" s="43"/>
+      <c r="D24" s="63">
+        <v>0</v>
+      </c>
+      <c r="E24" s="63">
+        <v>0</v>
+      </c>
       <c r="F24" s="44"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
@@ -6254,18 +6321,20 @@
       <c r="M24" s="44"/>
       <c r="N24" s="44"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A25" s="67"/>
-      <c r="B25" s="62" t="s">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="66"/>
+      <c r="B25" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="64">
-        <v>0</v>
-      </c>
-      <c r="E25" s="43"/>
+      <c r="D25" s="63">
+        <v>0</v>
+      </c>
+      <c r="E25" s="63">
+        <v>0</v>
+      </c>
       <c r="F25" s="44"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
@@ -6276,18 +6345,20 @@
       <c r="M25" s="44"/>
       <c r="N25" s="44"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A26" s="67"/>
-      <c r="B26" s="62" t="s">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="66"/>
+      <c r="B26" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="64">
-        <v>0</v>
-      </c>
-      <c r="E26" s="43"/>
+      <c r="D26" s="63">
+        <v>0</v>
+      </c>
+      <c r="E26" s="63">
+        <v>0</v>
+      </c>
       <c r="F26" s="44"/>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
@@ -6298,18 +6369,20 @@
       <c r="M26" s="44"/>
       <c r="N26" s="44"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A27" s="67"/>
-      <c r="B27" s="62" t="s">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="66"/>
+      <c r="B27" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="64">
-        <v>0</v>
-      </c>
-      <c r="E27" s="43"/>
+      <c r="D27" s="63">
+        <v>0</v>
+      </c>
+      <c r="E27" s="63">
+        <v>0</v>
+      </c>
       <c r="F27" s="44"/>
       <c r="G27" s="44"/>
       <c r="H27" s="44"/>
@@ -6320,18 +6393,20 @@
       <c r="M27" s="44"/>
       <c r="N27" s="44"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A28" s="67"/>
-      <c r="B28" s="62" t="s">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="66"/>
+      <c r="B28" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="64">
-        <v>0</v>
-      </c>
-      <c r="E28" s="43"/>
+      <c r="D28" s="63">
+        <v>0</v>
+      </c>
+      <c r="E28" s="63">
+        <v>0</v>
+      </c>
       <c r="F28" s="44"/>
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
@@ -6342,18 +6417,20 @@
       <c r="M28" s="44"/>
       <c r="N28" s="44"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A29" s="67"/>
-      <c r="B29" s="62" t="s">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="66"/>
+      <c r="B29" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="64">
-        <v>0</v>
-      </c>
-      <c r="E29" s="43"/>
+      <c r="D29" s="63">
+        <v>0</v>
+      </c>
+      <c r="E29" s="63">
+        <v>0</v>
+      </c>
       <c r="F29" s="44"/>
       <c r="G29" s="44"/>
       <c r="H29" s="44"/>
@@ -6364,18 +6441,20 @@
       <c r="M29" s="44"/>
       <c r="N29" s="44"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A30" s="67"/>
-      <c r="B30" s="62" t="s">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="66"/>
+      <c r="B30" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="64">
-        <v>0</v>
-      </c>
-      <c r="E30" s="43"/>
+      <c r="D30" s="63">
+        <v>0</v>
+      </c>
+      <c r="E30" s="63">
+        <v>0</v>
+      </c>
       <c r="F30" s="44"/>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
@@ -6386,18 +6465,20 @@
       <c r="M30" s="44"/>
       <c r="N30" s="44"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A31" s="67"/>
-      <c r="B31" s="62" t="s">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="66"/>
+      <c r="B31" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="64">
-        <v>0</v>
-      </c>
-      <c r="E31" s="43"/>
+      <c r="D31" s="63">
+        <v>0</v>
+      </c>
+      <c r="E31" s="63">
+        <v>0</v>
+      </c>
       <c r="F31" s="44"/>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
@@ -6408,18 +6489,20 @@
       <c r="M31" s="44"/>
       <c r="N31" s="44"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A32" s="67"/>
-      <c r="B32" s="62" t="s">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="66"/>
+      <c r="B32" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="63" t="s">
+      <c r="C32" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="64">
-        <v>0</v>
-      </c>
-      <c r="E32" s="43"/>
+      <c r="D32" s="63">
+        <v>0</v>
+      </c>
+      <c r="E32" s="63">
+        <v>0</v>
+      </c>
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
@@ -6430,18 +6513,20 @@
       <c r="M32" s="44"/>
       <c r="N32" s="44"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A33" s="67"/>
-      <c r="B33" s="62" t="s">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="66"/>
+      <c r="B33" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C33" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="64">
-        <v>0</v>
-      </c>
-      <c r="E33" s="43"/>
+      <c r="D33" s="63">
+        <v>0</v>
+      </c>
+      <c r="E33" s="63">
+        <v>0</v>
+      </c>
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
@@ -6452,18 +6537,20 @@
       <c r="M33" s="44"/>
       <c r="N33" s="44"/>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A34" s="67"/>
-      <c r="B34" s="62" t="s">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="66"/>
+      <c r="B34" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="C34" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="64">
-        <v>0</v>
-      </c>
-      <c r="E34" s="43"/>
+      <c r="D34" s="63">
+        <v>0</v>
+      </c>
+      <c r="E34" s="63">
+        <v>0</v>
+      </c>
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
       <c r="H34" s="44"/>
@@ -6474,18 +6561,20 @@
       <c r="M34" s="44"/>
       <c r="N34" s="44"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A35" s="67"/>
-      <c r="B35" s="62" t="s">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="66"/>
+      <c r="B35" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="63" t="s">
+      <c r="C35" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="64">
-        <v>0</v>
-      </c>
-      <c r="E35" s="43"/>
+      <c r="D35" s="63">
+        <v>0</v>
+      </c>
+      <c r="E35" s="63">
+        <v>0</v>
+      </c>
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
@@ -6496,18 +6585,20 @@
       <c r="M35" s="44"/>
       <c r="N35" s="44"/>
     </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A36" s="67"/>
-      <c r="B36" s="62" t="s">
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="66"/>
+      <c r="B36" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="63" t="s">
+      <c r="C36" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="64">
-        <v>0</v>
-      </c>
-      <c r="E36" s="43"/>
+      <c r="D36" s="63">
+        <v>0</v>
+      </c>
+      <c r="E36" s="63">
+        <v>0</v>
+      </c>
       <c r="F36" s="44"/>
       <c r="G36" s="44"/>
       <c r="H36" s="44"/>
@@ -6518,18 +6609,20 @@
       <c r="M36" s="44"/>
       <c r="N36" s="44"/>
     </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A37" s="67"/>
-      <c r="B37" s="62" t="s">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="66"/>
+      <c r="B37" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="64">
-        <v>0</v>
-      </c>
-      <c r="E37" s="43"/>
+      <c r="D37" s="63">
+        <v>0</v>
+      </c>
+      <c r="E37" s="63">
+        <v>0</v>
+      </c>
       <c r="F37" s="44"/>
       <c r="G37" s="44"/>
       <c r="H37" s="44"/>
@@ -6540,18 +6633,20 @@
       <c r="M37" s="44"/>
       <c r="N37" s="44"/>
     </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A38" s="67"/>
-      <c r="B38" s="62" t="s">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="66"/>
+      <c r="B38" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="63" t="s">
+      <c r="C38" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="64">
-        <v>0</v>
-      </c>
-      <c r="E38" s="43"/>
+      <c r="D38" s="63">
+        <v>0</v>
+      </c>
+      <c r="E38" s="63">
+        <v>0</v>
+      </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44"/>
       <c r="H38" s="44"/>
@@ -6562,18 +6657,20 @@
       <c r="M38" s="44"/>
       <c r="N38" s="44"/>
     </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A39" s="67"/>
-      <c r="B39" s="62" t="s">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="66"/>
+      <c r="B39" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="64">
-        <v>0</v>
-      </c>
-      <c r="E39" s="43"/>
+      <c r="D39" s="63">
+        <v>0</v>
+      </c>
+      <c r="E39" s="63">
+        <v>0</v>
+      </c>
       <c r="F39" s="44"/>
       <c r="G39" s="44"/>
       <c r="H39" s="44"/>
@@ -6584,18 +6681,20 @@
       <c r="M39" s="44"/>
       <c r="N39" s="44"/>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A40" s="67"/>
-      <c r="B40" s="62" t="s">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="66"/>
+      <c r="B40" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="63" t="s">
+      <c r="C40" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="64">
-        <v>0</v>
-      </c>
-      <c r="E40" s="43"/>
+      <c r="D40" s="63">
+        <v>0</v>
+      </c>
+      <c r="E40" s="63">
+        <v>0</v>
+      </c>
       <c r="F40" s="44"/>
       <c r="G40" s="44"/>
       <c r="H40" s="44"/>
@@ -6606,18 +6705,20 @@
       <c r="M40" s="44"/>
       <c r="N40" s="44"/>
     </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A41" s="67"/>
-      <c r="B41" s="62" t="s">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="66"/>
+      <c r="B41" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="64">
-        <v>0</v>
-      </c>
-      <c r="E41" s="43"/>
+      <c r="D41" s="63">
+        <v>0</v>
+      </c>
+      <c r="E41" s="63">
+        <v>0</v>
+      </c>
       <c r="F41" s="44"/>
       <c r="G41" s="44"/>
       <c r="H41" s="44"/>
@@ -6628,18 +6729,20 @@
       <c r="M41" s="44"/>
       <c r="N41" s="44"/>
     </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A42" s="67"/>
-      <c r="B42" s="62" t="s">
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="66"/>
+      <c r="B42" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="64">
-        <v>0</v>
-      </c>
-      <c r="E42" s="43"/>
+      <c r="D42" s="63">
+        <v>0</v>
+      </c>
+      <c r="E42" s="63">
+        <v>0</v>
+      </c>
       <c r="F42" s="44"/>
       <c r="G42" s="44"/>
       <c r="H42" s="44"/>
@@ -6650,18 +6753,20 @@
       <c r="M42" s="44"/>
       <c r="N42" s="44"/>
     </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A43" s="67"/>
-      <c r="B43" s="62" t="s">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="66"/>
+      <c r="B43" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="64">
-        <v>0</v>
-      </c>
-      <c r="E43" s="43"/>
+      <c r="D43" s="63">
+        <v>0</v>
+      </c>
+      <c r="E43" s="63">
+        <v>0</v>
+      </c>
       <c r="F43" s="44"/>
       <c r="G43" s="44"/>
       <c r="H43" s="44"/>
@@ -6672,18 +6777,20 @@
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
     </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A44" s="67"/>
-      <c r="B44" s="62" t="s">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="66"/>
+      <c r="B44" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="63" t="s">
+      <c r="C44" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="64">
-        <v>0</v>
-      </c>
-      <c r="E44" s="43"/>
+      <c r="D44" s="63">
+        <v>0</v>
+      </c>
+      <c r="E44" s="63">
+        <v>0</v>
+      </c>
       <c r="F44" s="44"/>
       <c r="G44" s="44"/>
       <c r="H44" s="44"/>
@@ -6694,18 +6801,20 @@
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A45" s="67"/>
-      <c r="B45" s="62" t="s">
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="66"/>
+      <c r="B45" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="63" t="s">
+      <c r="C45" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="64">
-        <v>0</v>
-      </c>
-      <c r="E45" s="43"/>
+      <c r="D45" s="63">
+        <v>0</v>
+      </c>
+      <c r="E45" s="63">
+        <v>0</v>
+      </c>
       <c r="F45" s="44"/>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
@@ -6716,18 +6825,20 @@
       <c r="M45" s="44"/>
       <c r="N45" s="44"/>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A46" s="67"/>
-      <c r="B46" s="62" t="s">
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="66"/>
+      <c r="B46" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="63" t="s">
+      <c r="C46" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="64">
-        <v>0</v>
-      </c>
-      <c r="E46" s="43"/>
+      <c r="D46" s="63">
+        <v>0</v>
+      </c>
+      <c r="E46" s="63">
+        <v>0</v>
+      </c>
       <c r="F46" s="44"/>
       <c r="G46" s="44"/>
       <c r="H46" s="44"/>
@@ -6738,18 +6849,20 @@
       <c r="M46" s="44"/>
       <c r="N46" s="44"/>
     </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A47" s="67"/>
-      <c r="B47" s="62" t="s">
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="66"/>
+      <c r="B47" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="63" t="s">
+      <c r="C47" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="64">
-        <v>0</v>
-      </c>
-      <c r="E47" s="43"/>
+      <c r="D47" s="63">
+        <v>0</v>
+      </c>
+      <c r="E47" s="63">
+        <v>0</v>
+      </c>
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
@@ -6760,18 +6873,20 @@
       <c r="M47" s="44"/>
       <c r="N47" s="44"/>
     </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A48" s="67"/>
-      <c r="B48" s="62" t="s">
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="66"/>
+      <c r="B48" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="63" t="s">
+      <c r="C48" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="64">
-        <v>0</v>
-      </c>
-      <c r="E48" s="43"/>
+      <c r="D48" s="63">
+        <v>0</v>
+      </c>
+      <c r="E48" s="63">
+        <v>0</v>
+      </c>
       <c r="F48" s="44"/>
       <c r="G48" s="44"/>
       <c r="H48" s="44"/>
@@ -6782,18 +6897,20 @@
       <c r="M48" s="44"/>
       <c r="N48" s="44"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A49" s="67"/>
-      <c r="B49" s="62" t="s">
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="66"/>
+      <c r="B49" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="63" t="s">
+      <c r="C49" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="64">
-        <v>0</v>
-      </c>
-      <c r="E49" s="43"/>
+      <c r="D49" s="63">
+        <v>0</v>
+      </c>
+      <c r="E49" s="63">
+        <v>0</v>
+      </c>
       <c r="F49" s="44"/>
       <c r="G49" s="44"/>
       <c r="H49" s="44"/>
@@ -6804,18 +6921,20 @@
       <c r="M49" s="44"/>
       <c r="N49" s="44"/>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A50" s="67"/>
-      <c r="B50" s="62" t="s">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="66"/>
+      <c r="B50" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="63" t="s">
+      <c r="C50" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="64">
-        <v>0</v>
-      </c>
-      <c r="E50" s="43"/>
+      <c r="D50" s="63">
+        <v>0</v>
+      </c>
+      <c r="E50" s="63">
+        <v>0</v>
+      </c>
       <c r="F50" s="44"/>
       <c r="G50" s="44"/>
       <c r="H50" s="44"/>
@@ -6826,18 +6945,20 @@
       <c r="M50" s="44"/>
       <c r="N50" s="44"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A51" s="67"/>
-      <c r="B51" s="62" t="s">
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="66"/>
+      <c r="B51" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="63" t="s">
+      <c r="C51" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="64">
-        <v>0</v>
-      </c>
-      <c r="E51" s="43"/>
+      <c r="D51" s="63">
+        <v>0</v>
+      </c>
+      <c r="E51" s="63">
+        <v>0</v>
+      </c>
       <c r="F51" s="44"/>
       <c r="G51" s="44"/>
       <c r="H51" s="44"/>
@@ -6848,18 +6969,20 @@
       <c r="M51" s="44"/>
       <c r="N51" s="44"/>
     </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A52" s="67"/>
-      <c r="B52" s="62" t="s">
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="66"/>
+      <c r="B52" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="63" t="s">
+      <c r="C52" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="64">
-        <v>0</v>
-      </c>
-      <c r="E52" s="43"/>
+      <c r="D52" s="63">
+        <v>0</v>
+      </c>
+      <c r="E52" s="63">
+        <v>0</v>
+      </c>
       <c r="F52" s="44"/>
       <c r="G52" s="44"/>
       <c r="H52" s="44"/>
@@ -6870,18 +6993,20 @@
       <c r="M52" s="44"/>
       <c r="N52" s="44"/>
     </row>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A53" s="67"/>
-      <c r="B53" s="62" t="s">
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="66"/>
+      <c r="B53" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="63" t="s">
+      <c r="C53" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="64">
-        <v>0</v>
-      </c>
-      <c r="E53" s="43"/>
+      <c r="D53" s="63">
+        <v>0</v>
+      </c>
+      <c r="E53" s="63">
+        <v>0</v>
+      </c>
       <c r="F53" s="44"/>
       <c r="G53" s="44"/>
       <c r="H53" s="44"/>
@@ -6892,18 +7017,20 @@
       <c r="M53" s="44"/>
       <c r="N53" s="44"/>
     </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A54" s="67"/>
-      <c r="B54" s="62" t="s">
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="66"/>
+      <c r="B54" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="63" t="s">
+      <c r="C54" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="64">
-        <v>0</v>
-      </c>
-      <c r="E54" s="43"/>
+      <c r="D54" s="63">
+        <v>0</v>
+      </c>
+      <c r="E54" s="63">
+        <v>0</v>
+      </c>
       <c r="F54" s="44"/>
       <c r="G54" s="44"/>
       <c r="H54" s="44"/>
@@ -6914,18 +7041,20 @@
       <c r="M54" s="44"/>
       <c r="N54" s="44"/>
     </row>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A55" s="67"/>
-      <c r="B55" s="62" t="s">
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="66"/>
+      <c r="B55" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="63" t="s">
+      <c r="C55" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="64">
-        <v>0</v>
-      </c>
-      <c r="E55" s="43"/>
+      <c r="D55" s="63">
+        <v>0</v>
+      </c>
+      <c r="E55" s="63">
+        <v>0</v>
+      </c>
       <c r="F55" s="44"/>
       <c r="G55" s="44"/>
       <c r="H55" s="44"/>
@@ -6936,18 +7065,20 @@
       <c r="M55" s="44"/>
       <c r="N55" s="44"/>
     </row>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A56" s="67"/>
-      <c r="B56" s="62" t="s">
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="66"/>
+      <c r="B56" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="63" t="s">
+      <c r="C56" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="64">
-        <v>0</v>
-      </c>
-      <c r="E56" s="43"/>
+      <c r="D56" s="63">
+        <v>0</v>
+      </c>
+      <c r="E56" s="63">
+        <v>0</v>
+      </c>
       <c r="F56" s="44"/>
       <c r="G56" s="44"/>
       <c r="H56" s="44"/>
@@ -6958,18 +7089,20 @@
       <c r="M56" s="44"/>
       <c r="N56" s="44"/>
     </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A57" s="67"/>
-      <c r="B57" s="62" t="s">
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="66"/>
+      <c r="B57" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="63" t="s">
+      <c r="C57" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="64">
-        <v>0</v>
-      </c>
-      <c r="E57" s="43"/>
+      <c r="D57" s="63">
+        <v>0</v>
+      </c>
+      <c r="E57" s="63">
+        <v>0</v>
+      </c>
       <c r="F57" s="44"/>
       <c r="G57" s="44"/>
       <c r="H57" s="44"/>
@@ -6980,18 +7113,20 @@
       <c r="M57" s="44"/>
       <c r="N57" s="44"/>
     </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A58" s="67"/>
-      <c r="B58" s="62" t="s">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="66"/>
+      <c r="B58" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="63" t="s">
+      <c r="C58" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="64">
-        <v>0</v>
-      </c>
-      <c r="E58" s="43"/>
+      <c r="D58" s="63">
+        <v>0</v>
+      </c>
+      <c r="E58" s="63">
+        <v>0</v>
+      </c>
       <c r="F58" s="44"/>
       <c r="G58" s="44"/>
       <c r="H58" s="44"/>
@@ -7002,12 +7137,12 @@
       <c r="M58" s="44"/>
       <c r="N58" s="44"/>
     </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A59" s="67"/>
-      <c r="B59" s="68"/>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="66"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="44"/>
-      <c r="D59" s="69"/>
-      <c r="E59" s="43"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="76"/>
       <c r="F59" s="44"/>
       <c r="G59" s="44"/>
       <c r="H59" s="44"/>
@@ -7018,12 +7153,12 @@
       <c r="M59" s="44"/>
       <c r="N59" s="44"/>
     </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A60" s="67"/>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="66"/>
       <c r="B60" s="43"/>
       <c r="C60" s="44"/>
-      <c r="D60" s="69"/>
-      <c r="E60" s="43"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="76"/>
       <c r="F60" s="44"/>
       <c r="G60" s="44"/>
       <c r="H60" s="44"/>
@@ -7034,12 +7169,12 @@
       <c r="M60" s="44"/>
       <c r="N60" s="44"/>
     </row>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A61" s="67"/>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="66"/>
       <c r="B61" s="43"/>
       <c r="C61" s="44"/>
-      <c r="D61" s="69"/>
-      <c r="E61" s="43"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="76"/>
       <c r="F61" s="44"/>
       <c r="G61" s="44"/>
       <c r="H61" s="44"/>
@@ -7050,12 +7185,12 @@
       <c r="M61" s="44"/>
       <c r="N61" s="44"/>
     </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A62" s="67"/>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="66"/>
       <c r="B62" s="43"/>
       <c r="C62" s="44"/>
-      <c r="D62" s="69"/>
-      <c r="E62" s="43"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="76"/>
       <c r="F62" s="44"/>
       <c r="G62" s="44"/>
       <c r="H62" s="44"/>
@@ -7066,12 +7201,12 @@
       <c r="M62" s="44"/>
       <c r="N62" s="44"/>
     </row>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A63" s="67"/>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="66"/>
       <c r="B63" s="43"/>
       <c r="C63" s="44"/>
-      <c r="D63" s="69"/>
-      <c r="E63" s="43"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="76"/>
       <c r="F63" s="44"/>
       <c r="G63" s="44"/>
       <c r="H63" s="44"/>
@@ -7082,12 +7217,12 @@
       <c r="M63" s="44"/>
       <c r="N63" s="44"/>
     </row>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A64" s="67"/>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="66"/>
       <c r="B64" s="43"/>
       <c r="C64" s="44"/>
-      <c r="D64" s="69"/>
-      <c r="E64" s="43"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="76"/>
       <c r="F64" s="44"/>
       <c r="G64" s="44"/>
       <c r="H64" s="44"/>
@@ -7098,12 +7233,12 @@
       <c r="M64" s="44"/>
       <c r="N64" s="44"/>
     </row>
-    <row r="65" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A65" s="67"/>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="66"/>
       <c r="B65" s="43"/>
       <c r="C65" s="44"/>
-      <c r="D65" s="69"/>
-      <c r="E65" s="43"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="76"/>
       <c r="F65" s="44"/>
       <c r="G65" s="44"/>
       <c r="H65" s="44"/>
@@ -7114,12 +7249,12 @@
       <c r="M65" s="44"/>
       <c r="N65" s="44"/>
     </row>
-    <row r="66" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A66" s="67"/>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="66"/>
       <c r="B66" s="43"/>
       <c r="C66" s="44"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="43"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="76"/>
       <c r="F66" s="44"/>
       <c r="G66" s="44"/>
       <c r="H66" s="44"/>
@@ -7130,12 +7265,12 @@
       <c r="M66" s="44"/>
       <c r="N66" s="44"/>
     </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A67" s="67"/>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="66"/>
       <c r="B67" s="43"/>
       <c r="C67" s="44"/>
-      <c r="D67" s="64"/>
-      <c r="E67" s="43"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="76"/>
       <c r="F67" s="44"/>
       <c r="G67" s="44"/>
       <c r="H67" s="44"/>
@@ -7146,12 +7281,12 @@
       <c r="M67" s="44"/>
       <c r="N67" s="44"/>
     </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A68" s="67"/>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="66"/>
       <c r="B68" s="43"/>
       <c r="C68" s="44"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="43"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="76"/>
       <c r="F68" s="44"/>
       <c r="G68" s="44"/>
       <c r="H68" s="44"/>
@@ -7162,12 +7297,12 @@
       <c r="M68" s="44"/>
       <c r="N68" s="44"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A69" s="67"/>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="66"/>
       <c r="B69" s="43"/>
       <c r="C69" s="44"/>
-      <c r="D69" s="64"/>
-      <c r="E69" s="43"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="76"/>
       <c r="F69" s="44"/>
       <c r="G69" s="44"/>
       <c r="H69" s="44"/>
@@ -7178,12 +7313,12 @@
       <c r="M69" s="44"/>
       <c r="N69" s="44"/>
     </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A70" s="67"/>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="66"/>
       <c r="B70" s="43"/>
       <c r="C70" s="44"/>
-      <c r="D70" s="64"/>
-      <c r="E70" s="43"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="76"/>
       <c r="F70" s="44"/>
       <c r="G70" s="44"/>
       <c r="H70" s="44"/>
@@ -7194,12 +7329,12 @@
       <c r="M70" s="44"/>
       <c r="N70" s="44"/>
     </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A71" s="67"/>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="66"/>
       <c r="B71" s="43"/>
       <c r="C71" s="44"/>
-      <c r="D71" s="64"/>
-      <c r="E71" s="43"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="76"/>
       <c r="F71" s="44"/>
       <c r="G71" s="44"/>
       <c r="H71" s="44"/>
@@ -7210,12 +7345,12 @@
       <c r="M71" s="44"/>
       <c r="N71" s="44"/>
     </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A72" s="67"/>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="66"/>
       <c r="B72" s="43"/>
       <c r="C72" s="44"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="43"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="76"/>
       <c r="F72" s="44"/>
       <c r="G72" s="44"/>
       <c r="H72" s="44"/>
@@ -7226,12 +7361,12 @@
       <c r="M72" s="44"/>
       <c r="N72" s="44"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A73" s="67"/>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="66"/>
       <c r="B73" s="43"/>
       <c r="C73" s="44"/>
-      <c r="D73" s="64"/>
-      <c r="E73" s="43"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="76"/>
       <c r="F73" s="44"/>
       <c r="G73" s="44"/>
       <c r="H73" s="44"/>
@@ -7242,12 +7377,12 @@
       <c r="M73" s="44"/>
       <c r="N73" s="44"/>
     </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A74" s="67"/>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="66"/>
       <c r="B74" s="43"/>
       <c r="C74" s="44"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="43"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="76"/>
       <c r="F74" s="44"/>
       <c r="G74" s="44"/>
       <c r="H74" s="44"/>
@@ -7258,12 +7393,12 @@
       <c r="M74" s="44"/>
       <c r="N74" s="44"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A75" s="67"/>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="66"/>
       <c r="B75" s="43"/>
       <c r="C75" s="44"/>
-      <c r="D75" s="64"/>
-      <c r="E75" s="43"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="76"/>
       <c r="F75" s="44"/>
       <c r="G75" s="44"/>
       <c r="H75" s="44"/>
@@ -7274,12 +7409,12 @@
       <c r="M75" s="44"/>
       <c r="N75" s="44"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A76" s="67"/>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="66"/>
       <c r="B76" s="43"/>
       <c r="C76" s="44"/>
-      <c r="D76" s="64"/>
-      <c r="E76" s="43"/>
+      <c r="D76" s="63"/>
+      <c r="E76" s="76"/>
       <c r="F76" s="44"/>
       <c r="G76" s="44"/>
       <c r="H76" s="44"/>
@@ -7290,12 +7425,12 @@
       <c r="M76" s="44"/>
       <c r="N76" s="44"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A77" s="67"/>
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="66"/>
       <c r="B77" s="43"/>
       <c r="C77" s="44"/>
-      <c r="D77" s="64"/>
-      <c r="E77" s="43"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="76"/>
       <c r="F77" s="44"/>
       <c r="G77" s="44"/>
       <c r="H77" s="44"/>
@@ -7306,12 +7441,12 @@
       <c r="M77" s="44"/>
       <c r="N77" s="44"/>
     </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A78" s="67"/>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="66"/>
       <c r="B78" s="43"/>
       <c r="C78" s="44"/>
-      <c r="D78" s="64"/>
-      <c r="E78" s="43"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="76"/>
       <c r="F78" s="44"/>
       <c r="G78" s="44"/>
       <c r="H78" s="44"/>
@@ -7322,12 +7457,12 @@
       <c r="M78" s="44"/>
       <c r="N78" s="44"/>
     </row>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A79" s="67"/>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="66"/>
       <c r="B79" s="43"/>
       <c r="C79" s="44"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="43"/>
+      <c r="D79" s="63"/>
+      <c r="E79" s="76"/>
       <c r="F79" s="44"/>
       <c r="G79" s="44"/>
       <c r="H79" s="44"/>
@@ -7338,12 +7473,12 @@
       <c r="M79" s="44"/>
       <c r="N79" s="44"/>
     </row>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A80" s="67"/>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="66"/>
       <c r="B80" s="43"/>
       <c r="C80" s="44"/>
-      <c r="D80" s="64"/>
-      <c r="E80" s="43"/>
+      <c r="D80" s="63"/>
+      <c r="E80" s="76"/>
       <c r="F80" s="44"/>
       <c r="G80" s="44"/>
       <c r="H80" s="44"/>
@@ -7354,12 +7489,12 @@
       <c r="M80" s="44"/>
       <c r="N80" s="44"/>
     </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A81" s="67"/>
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="66"/>
       <c r="B81" s="43"/>
       <c r="C81" s="44"/>
-      <c r="D81" s="64"/>
-      <c r="E81" s="43"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="76"/>
       <c r="F81" s="44"/>
       <c r="G81" s="44"/>
       <c r="H81" s="44"/>
@@ -7370,12 +7505,12 @@
       <c r="M81" s="44"/>
       <c r="N81" s="44"/>
     </row>
-    <row r="82" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A82" s="67"/>
+    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="66"/>
       <c r="B82" s="43"/>
       <c r="C82" s="44"/>
-      <c r="D82" s="64"/>
-      <c r="E82" s="43"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="76"/>
       <c r="F82" s="44"/>
       <c r="G82" s="44"/>
       <c r="H82" s="44"/>
@@ -7386,12 +7521,12 @@
       <c r="M82" s="44"/>
       <c r="N82" s="44"/>
     </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A83" s="67"/>
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="66"/>
       <c r="B83" s="43"/>
       <c r="C83" s="44"/>
-      <c r="D83" s="64"/>
-      <c r="E83" s="43"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="76"/>
       <c r="F83" s="44"/>
       <c r="G83" s="44"/>
       <c r="H83" s="44"/>
@@ -7402,12 +7537,12 @@
       <c r="M83" s="44"/>
       <c r="N83" s="44"/>
     </row>
-    <row r="84" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A84" s="67"/>
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="66"/>
       <c r="B84" s="43"/>
       <c r="C84" s="44"/>
-      <c r="D84" s="64"/>
-      <c r="E84" s="43"/>
+      <c r="D84" s="63"/>
+      <c r="E84" s="76"/>
       <c r="F84" s="44"/>
       <c r="G84" s="44"/>
       <c r="H84" s="44"/>
@@ -7418,12 +7553,12 @@
       <c r="M84" s="44"/>
       <c r="N84" s="44"/>
     </row>
-    <row r="85" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A85" s="67"/>
+    <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="66"/>
       <c r="B85" s="43"/>
       <c r="C85" s="44"/>
-      <c r="D85" s="64"/>
-      <c r="E85" s="43"/>
+      <c r="D85" s="63"/>
+      <c r="E85" s="76"/>
       <c r="F85" s="44"/>
       <c r="G85" s="44"/>
       <c r="H85" s="44"/>
@@ -7434,12 +7569,12 @@
       <c r="M85" s="44"/>
       <c r="N85" s="44"/>
     </row>
-    <row r="86" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A86" s="67"/>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="66"/>
       <c r="B86" s="43"/>
       <c r="C86" s="44"/>
-      <c r="D86" s="64"/>
-      <c r="E86" s="43"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="76"/>
       <c r="F86" s="44"/>
       <c r="G86" s="44"/>
       <c r="H86" s="44"/>
@@ -7450,12 +7585,12 @@
       <c r="M86" s="44"/>
       <c r="N86" s="44"/>
     </row>
-    <row r="87" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A87" s="67"/>
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="66"/>
       <c r="B87" s="43"/>
       <c r="C87" s="44"/>
-      <c r="D87" s="64"/>
-      <c r="E87" s="43"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="76"/>
       <c r="F87" s="44"/>
       <c r="G87" s="44"/>
       <c r="H87" s="44"/>
@@ -7466,12 +7601,12 @@
       <c r="M87" s="44"/>
       <c r="N87" s="44"/>
     </row>
-    <row r="88" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A88" s="67"/>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="66"/>
       <c r="B88" s="43"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="64"/>
-      <c r="E88" s="43"/>
+      <c r="D88" s="63"/>
+      <c r="E88" s="76"/>
       <c r="F88" s="44"/>
       <c r="G88" s="44"/>
       <c r="H88" s="44"/>
@@ -7482,12 +7617,12 @@
       <c r="M88" s="44"/>
       <c r="N88" s="44"/>
     </row>
-    <row r="89" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A89" s="67"/>
+    <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="66"/>
       <c r="B89" s="43"/>
       <c r="C89" s="44"/>
-      <c r="D89" s="64"/>
-      <c r="E89" s="43"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="76"/>
       <c r="F89" s="44"/>
       <c r="G89" s="44"/>
       <c r="H89" s="44"/>
@@ -7498,12 +7633,12 @@
       <c r="M89" s="44"/>
       <c r="N89" s="44"/>
     </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A90" s="67"/>
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="66"/>
       <c r="B90" s="43"/>
       <c r="C90" s="44"/>
-      <c r="D90" s="64"/>
-      <c r="E90" s="43"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="76"/>
       <c r="F90" s="44"/>
       <c r="G90" s="44"/>
       <c r="H90" s="44"/>
@@ -7514,12 +7649,12 @@
       <c r="M90" s="44"/>
       <c r="N90" s="44"/>
     </row>
-    <row r="91" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A91" s="67"/>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="66"/>
       <c r="B91" s="43"/>
       <c r="C91" s="44"/>
-      <c r="D91" s="64"/>
-      <c r="E91" s="43"/>
+      <c r="D91" s="63"/>
+      <c r="E91" s="76"/>
       <c r="F91" s="44"/>
       <c r="G91" s="44"/>
       <c r="H91" s="44"/>
@@ -7530,12 +7665,12 @@
       <c r="M91" s="44"/>
       <c r="N91" s="44"/>
     </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A92" s="67"/>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="66"/>
       <c r="B92" s="43"/>
       <c r="C92" s="44"/>
-      <c r="D92" s="64"/>
-      <c r="E92" s="43"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="76"/>
       <c r="F92" s="44"/>
       <c r="G92" s="44"/>
       <c r="H92" s="44"/>
@@ -7546,12 +7681,12 @@
       <c r="M92" s="44"/>
       <c r="N92" s="44"/>
     </row>
-    <row r="93" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A93" s="67"/>
+    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="66"/>
       <c r="B93" s="43"/>
       <c r="C93" s="44"/>
-      <c r="D93" s="64"/>
-      <c r="E93" s="43"/>
+      <c r="D93" s="63"/>
+      <c r="E93" s="76"/>
       <c r="F93" s="44"/>
       <c r="G93" s="44"/>
       <c r="H93" s="44"/>
@@ -7562,12 +7697,12 @@
       <c r="M93" s="44"/>
       <c r="N93" s="44"/>
     </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A94" s="67"/>
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="66"/>
       <c r="B94" s="43"/>
       <c r="C94" s="44"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="43"/>
+      <c r="D94" s="63"/>
+      <c r="E94" s="76"/>
       <c r="F94" s="44"/>
       <c r="G94" s="44"/>
       <c r="H94" s="44"/>
@@ -7578,12 +7713,12 @@
       <c r="M94" s="44"/>
       <c r="N94" s="44"/>
     </row>
-    <row r="95" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A95" s="67"/>
+    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="66"/>
       <c r="B95" s="43"/>
       <c r="C95" s="44"/>
-      <c r="D95" s="64"/>
-      <c r="E95" s="43"/>
+      <c r="D95" s="63"/>
+      <c r="E95" s="76"/>
       <c r="F95" s="44"/>
       <c r="G95" s="44"/>
       <c r="H95" s="44"/>
@@ -7594,12 +7729,12 @@
       <c r="M95" s="44"/>
       <c r="N95" s="44"/>
     </row>
-    <row r="96" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A96" s="67"/>
+    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="66"/>
       <c r="B96" s="43"/>
       <c r="C96" s="44"/>
-      <c r="D96" s="64"/>
-      <c r="E96" s="43"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="76"/>
       <c r="F96" s="44"/>
       <c r="G96" s="44"/>
       <c r="H96" s="44"/>
@@ -7610,12 +7745,12 @@
       <c r="M96" s="44"/>
       <c r="N96" s="44"/>
     </row>
-    <row r="97" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A97" s="70"/>
+    <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="69"/>
       <c r="B97" s="43"/>
       <c r="C97" s="44"/>
-      <c r="D97" s="64"/>
-      <c r="E97" s="43"/>
+      <c r="D97" s="63"/>
+      <c r="E97" s="76"/>
       <c r="F97" s="44"/>
       <c r="G97" s="44"/>
       <c r="H97" s="44"/>
@@ -7628,7 +7763,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>